<commit_message>
Added e2e flow with file downloading
</commit_message>
<xml_diff>
--- a/src/test/resources/file/testFile.xlsx
+++ b/src/test/resources/file/testFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr_Diachenko\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr_Diachenko\IdeaProjects\price-checker-web\price-checker-automation\src\test\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E50A36C-EC39-405D-A56E-86BA6416B6B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EF7911-8587-4910-AE49-11AB4980354A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FAEDBDEB-AD25-499B-A308-C36DF6309E40}"/>
   </bookViews>
@@ -33,9 +33,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>https://makeup.com.ua/product/742231/#/option/1714263/</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>https://makeup.com.ua/product/8383/#/option/463699/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/8383/#/option/463697/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/3173/#/option/401569/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/3173/#/option/401571/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/3173/#/option/401567/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/583163/#/option/1474529/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/215167/#/option/471781/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/11180/#/option/472003/</t>
+  </si>
+  <si>
+    <t>https://makeup.com.ua/product/11180/#/option/471999/</t>
+  </si>
+  <si>
+    <t>https://rozetka.com.ua/antonio_banderas_8411061636275/p2215142/</t>
+  </si>
+  <si>
+    <t>https://rozetka.com.ua/versace_img479/p11514465/</t>
+  </si>
+  <si>
+    <t>https://rozetka.com.ua/versace_8011003996025/p57030999/</t>
+  </si>
+  <si>
+    <t>https://rozetka.com.ua/creed_3508440505118/p69683708/</t>
+  </si>
+  <si>
+    <t>https://rozetka.com.ua/creed_3508441001114/p69673676/</t>
   </si>
 </sst>
 </file>
@@ -398,13 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74A8455-FDA3-47B2-B070-386EE3380138}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1"/>
+    <col min="1" max="1" width="67.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -412,9 +453,87 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" location="/option/1714263/" display="https://makeup.com.ua/product/742231/ - /option/1714263/" xr:uid="{C5F5061B-B4EE-421A-9693-DF74FCE4A074}"/>
+    <hyperlink ref="A1" r:id="rId1" location="/option/463699/" xr:uid="{C5F5061B-B4EE-421A-9693-DF74FCE4A074}"/>
+    <hyperlink ref="A2" r:id="rId2" location="/option/463697/" display="https://makeup.com.ua/product/8383/ - /option/463697/" xr:uid="{92394064-308A-47FB-A900-1255EB5EC19E}"/>
+    <hyperlink ref="A3" r:id="rId3" location="/option/401569/" display="https://makeup.com.ua/product/3173/ - /option/401569/" xr:uid="{7230F7A0-A677-421F-9101-4EC604994781}"/>
+    <hyperlink ref="A4" r:id="rId4" location="/option/401571/" display="https://makeup.com.ua/product/3173/ - /option/401571/" xr:uid="{5D74C649-2F08-48E9-8A74-635B4BDF6DBE}"/>
+    <hyperlink ref="A5" r:id="rId5" location="/option/401567/" display="https://makeup.com.ua/product/3173/ - /option/401567/" xr:uid="{A624DD96-EEE7-462F-B0A8-BDAF07FEDAD6}"/>
+    <hyperlink ref="A6" r:id="rId6" location="/option/1474529/" display="https://makeup.com.ua/product/583163/ - /option/1474529/" xr:uid="{852F8F3C-F8BB-4654-822C-33CBBF0F5339}"/>
+    <hyperlink ref="A7" r:id="rId7" location="/option/471781/" display="https://makeup.com.ua/product/215167/ - /option/471781/" xr:uid="{0D7EFD22-31DA-4C1C-BF5A-F2214B0463ED}"/>
+    <hyperlink ref="A8" r:id="rId8" location="/option/472003/" display="https://makeup.com.ua/product/11180/ - /option/472003/" xr:uid="{BDC7E684-C48E-4E0F-B95D-D40068482AFA}"/>
+    <hyperlink ref="A9" r:id="rId9" location="/option/471999/" display="https://makeup.com.ua/product/11180/ - /option/471999/" xr:uid="{76CF191D-64DD-483D-A1E2-8A62DFF94DF8}"/>
+    <hyperlink ref="A10" r:id="rId10" xr:uid="{9134F9A1-9405-4A26-8A0C-981996446C83}"/>
+    <hyperlink ref="A11" r:id="rId11" xr:uid="{2CBB21F9-5F93-454D-8467-6AA1AD031F3C}"/>
+    <hyperlink ref="A12" r:id="rId12" xr:uid="{E218495D-B207-4CBD-B75E-5372970A9522}"/>
+    <hyperlink ref="A13" r:id="rId13" xr:uid="{A6775779-7C98-4B4B-BADB-CA8E60D1472A}"/>
+    <hyperlink ref="A14" r:id="rId14" xr:uid="{17F4E638-9C40-4DD2-B4BB-CAAEF161F7B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>